<commit_message>
Auto push at 18:02:49
</commit_message>
<xml_diff>
--- a/semester 3/ais/accounting/problem solves/P1-1B_template.xlsx
+++ b/semester 3/ais/accounting/problem solves/P1-1B_template.xlsx
@@ -135,6 +135,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -155,6 +156,7 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -162,12 +164,14 @@
       <color rgb="FFC9211E"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -231,64 +235,68 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -478,14 +486,14 @@
   <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M18" activeCellId="0" sqref="M18"/>
+      <selection pane="topLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="24.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="24.67"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="2.88"/>
@@ -731,10 +739,10 @@
       <c r="F9" s="5"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8" t="n">
+      <c r="I9" s="8" t="n">
         <v>8500</v>
       </c>
+      <c r="J9" s="0"/>
       <c r="K9" s="8"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -783,7 +791,7 @@
         <v>3</v>
       </c>
       <c r="N11" s="9"/>
-      <c r="O11" s="0"/>
+      <c r="O11" s="13"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
@@ -833,7 +841,7 @@
         <v>4</v>
       </c>
       <c r="N13" s="9"/>
-      <c r="O13" s="0"/>
+      <c r="O13" s="13"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N14" s="8" t="s">
@@ -845,7 +853,7 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M15" s="13"/>
+      <c r="M15" s="14"/>
       <c r="N15" s="8" t="s">
         <v>21</v>
       </c>
@@ -868,12 +876,12 @@
       <c r="M18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="N18" s="14" t="str">
+      <c r="N18" s="15" t="str">
         <f aca="false">IF(O8=O16,"No error, it seems!","Error exists!")</f>
         <v>No error, it seems!</v>
       </c>
-      <c r="O18" s="14"/>
-      <c r="P18" s="0"/>
+      <c r="O18" s="15"/>
+      <c r="P18" s="13"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M19" s="3"/>
@@ -893,7 +901,7 @@
       </c>
       <c r="N22" s="8" t="n">
         <f aca="false">SUM(I4:I1000)</f>
-        <v>0</v>
+        <v>8500</v>
       </c>
       <c r="O22" s="3"/>
     </row>
@@ -903,12 +911,12 @@
       </c>
       <c r="N23" s="8" t="n">
         <f aca="false">SUM(J4:J1000)</f>
-        <v>5800</v>
+        <v>-2700</v>
       </c>
       <c r="O23" s="3"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M24" s="13" t="s">
+      <c r="M24" s="14" t="s">
         <v>27</v>
       </c>
       <c r="N24" s="11" t="n">
@@ -944,7 +952,7 @@
       <c r="O29" s="3"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M30" s="13" t="s">
+      <c r="M30" s="14" t="s">
         <v>31</v>
       </c>
       <c r="N30" s="11" t="n">
@@ -998,7 +1006,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="24.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="24.67"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="2.88"/>
@@ -1293,7 +1301,7 @@
         <v>3</v>
       </c>
       <c r="N11" s="9"/>
-      <c r="O11" s="0"/>
+      <c r="O11" s="13"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
@@ -1343,7 +1351,7 @@
         <v>4</v>
       </c>
       <c r="N13" s="9"/>
-      <c r="O13" s="0"/>
+      <c r="O13" s="13"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N14" s="8" t="s">
@@ -1355,7 +1363,7 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M15" s="13"/>
+      <c r="M15" s="14"/>
       <c r="N15" s="8" t="s">
         <v>21</v>
       </c>
@@ -1378,11 +1386,11 @@
       <c r="M18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="N18" s="14" t="str">
+      <c r="N18" s="15" t="str">
         <f aca="false">IF(O8=O16,"No error, it seems!","Error exists!")</f>
         <v>No error, it seems!</v>
       </c>
-      <c r="O18" s="14"/>
+      <c r="O18" s="15"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M19" s="3"/>
@@ -1417,7 +1425,7 @@
       <c r="O23" s="3"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M24" s="13" t="s">
+      <c r="M24" s="14" t="s">
         <v>27</v>
       </c>
       <c r="N24" s="11" t="n">
@@ -1453,7 +1461,7 @@
       <c r="O29" s="3"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M30" s="13" t="s">
+      <c r="M30" s="14" t="s">
         <v>31</v>
       </c>
       <c r="N30" s="11" t="n">

</xml_diff>

<commit_message>
Auto push at 21:01:25
</commit_message>
<xml_diff>
--- a/semester 3/ais/accounting/problem solves/P1-1B_template.xlsx
+++ b/semester 3/ais/accounting/problem solves/P1-1B_template.xlsx
@@ -284,19 +284,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -486,7 +486,7 @@
   <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
+      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -742,7 +742,7 @@
       <c r="I9" s="8" t="n">
         <v>8500</v>
       </c>
-      <c r="J9" s="0"/>
+      <c r="J9" s="12"/>
       <c r="K9" s="8"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -763,11 +763,11 @@
       <c r="K10" s="8" t="n">
         <v>-200</v>
       </c>
-      <c r="M10" s="12" t="s">
+      <c r="M10" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="N10" s="12"/>
-      <c r="O10" s="12"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
@@ -791,7 +791,7 @@
         <v>3</v>
       </c>
       <c r="N11" s="9"/>
-      <c r="O11" s="13"/>
+      <c r="O11" s="12"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
@@ -841,7 +841,7 @@
         <v>4</v>
       </c>
       <c r="N13" s="9"/>
-      <c r="O13" s="13"/>
+      <c r="O13" s="12"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N14" s="8" t="s">
@@ -881,7 +881,7 @@
         <v>No error, it seems!</v>
       </c>
       <c r="O18" s="15"/>
-      <c r="P18" s="13"/>
+      <c r="P18" s="12"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M19" s="3"/>
@@ -1273,11 +1273,11 @@
         <v>-1700</v>
       </c>
       <c r="K10" s="8"/>
-      <c r="M10" s="12" t="s">
+      <c r="M10" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="N10" s="12"/>
-      <c r="O10" s="12"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
@@ -1301,7 +1301,7 @@
         <v>3</v>
       </c>
       <c r="N11" s="9"/>
-      <c r="O11" s="13"/>
+      <c r="O11" s="12"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
@@ -1351,7 +1351,7 @@
         <v>4</v>
       </c>
       <c r="N13" s="9"/>
-      <c r="O13" s="13"/>
+      <c r="O13" s="12"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N14" s="8" t="s">

</xml_diff>